<commit_message>
fix: export Excel with token auth and improve error handling
</commit_message>
<xml_diff>
--- a/114_tkuim_final_project/backend/PyMoney_Export.xlsx
+++ b/114_tkuim_final_project/backend/PyMoney_Export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,103 +483,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>麥當勞</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="F2" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2026-01-11</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>expense</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>麥當勞</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>143</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2026-01-11</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>expense</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>藏壽司</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1040</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2026-01-11</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>expense</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Test VND</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="inlineStr">
         <is>
           <t>Cash</t>
         </is>

</xml_diff>